<commit_message>
Controller , user excel, model
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>sdflkj</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>sdflkj3333</t>
+  </si>
+  <si>
+    <t>sdfsd33</t>
   </si>
 </sst>
 </file>
@@ -85,7 +97,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -112,6 +124,22 @@
       </c>
       <c r="G1" t="s" s="1">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
showAllUserView return button - done
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>yoni@gmail.com</t>
+  </si>
+  <si>
+    <t>Lilach</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>lila</t>
+  </si>
+  <si>
+    <t>naor</t>
+  </si>
+  <si>
+    <t>lilach@gmail.com</t>
+  </si>
+  <si>
+    <t>054266</t>
   </si>
 </sst>
 </file>
@@ -448,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -584,6 +602,32 @@
       </c>
       <c r="H5" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
register validation - done
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{20BF12C9-F8FA-4229-AD2F-9ADDAF573433}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5AC386C8-A637-4487-B045-CC050EBA73CE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11385" windowWidth="21600" xWindow="2100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1080"/>
+    <workbookView windowHeight="11385" windowWidth="21600" xWindow="360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="645"/>
   </bookViews>
   <sheets>
     <sheet name="משתמשים" r:id="rId1" sheetId="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -122,51 +122,6 @@
     <t>vv</t>
   </si>
   <si>
-    <t>csc</t>
-  </si>
-  <si>
-    <t>efc</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>jkj</t>
-  </si>
-  <si>
-    <t>kjs</t>
-  </si>
-  <si>
-    <t>njj</t>
-  </si>
-  <si>
-    <t>jw</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>fg</t>
   </si>
   <si>
@@ -207,6 +162,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -566,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -702,138 +660,138 @@
       <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" t="n">
-        <v>1.0</v>
+      <c r="G6">
+        <v>1</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.0</v>
+        <v>38</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
       </c>
       <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="G8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1.0</v>
+        <v>44</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -841,79 +799,27 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G12" t="n">
         <v>1.0</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H14" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
show all apartment table
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{69D3C271-A0E3-49F7-B967-6AAC7E7B9156}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F0DD3-5E46-4410-9B21-E09FC1903E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="11385" windowWidth="21600" xWindow="4680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="555"/>
+    <workbookView xWindow="4680" yWindow="555" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="משתמשים" r:id="rId1" sheetId="1"/>
-    <sheet name="נכסים" r:id="rId2" sheetId="2"/>
+    <sheet name="משתמשים" sheetId="1" r:id="rId1"/>
+    <sheet name="נכסים" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -192,13 +192,15 @@
   </si>
   <si>
     <t>חיות</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,17 +234,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -259,10 +261,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -297,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -349,7 +351,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -460,21 +462,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -491,7 +493,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -543,23 +545,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,25 +721,25 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -745,22 +747,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -771,98 +773,46 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,7 +948,75 @@
         <v>56</v>
       </c>
     </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change data base and models
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F0DD3-5E46-4410-9B21-E09FC1903E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A5D152-DDFB-4E3F-8C5D-D011AC57A441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="555" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="משתמשים" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -41,12 +41,15 @@
     <t>טלפון</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>כמות חיפושים</t>
+  </si>
+  <si>
     <t>עיר</t>
   </si>
   <si>
@@ -155,19 +158,19 @@
     <t>gfh</t>
   </si>
   <si>
+    <t>Sap</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>ספיר</t>
+  </si>
+  <si>
+    <t>שמש</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>Sap</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>ספיר</t>
-  </si>
-  <si>
-    <t>שמש</t>
   </si>
   <si>
     <t>052</t>
@@ -553,15 +556,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,11 +586,8 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -606,120 +606,102 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
+      <c r="G2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
+      <c r="G3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="b">
+      <c r="G4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5">
         <v>547712222</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="b">
         <v>1</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
+        <v>38</v>
+      </c>
+      <c r="G6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
+        <v>44</v>
+      </c>
+      <c r="G7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -733,24 +715,21 @@
         <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="b">
+        <v>50</v>
+      </c>
+      <c r="G8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -759,41 +738,35 @@
         <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
         <v>49</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
       <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
+        <v>53</v>
+      </c>
+      <c r="G10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -804,112 +777,118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>222</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
-      </c>
       <c r="I2">
         <v>222</v>
       </c>
-      <c r="J2">
-        <v>222</v>
+      <c r="J2" t="s">
+        <v>56</v>
       </c>
       <c r="K2">
         <v>222</v>
@@ -941,79 +920,91 @@
       <c r="T2">
         <v>222</v>
       </c>
-      <c r="U2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>222</v>
+      </c>
+      <c r="V2">
+        <v>222</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="T3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="V3" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="W3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design + 2 classes in new window
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fastl\Documents\GitHub\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{87A5D152-DDFB-4E3F-8C5D-D011AC57A441}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{016AD528-8308-40D6-BE0F-DC27D0F488D7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="משתמשים" r:id="rId1" sheetId="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -198,6 +198,21 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Lilach</t>
+  </si>
+  <si>
+    <t>lilach</t>
+  </si>
+  <si>
+    <t>naor</t>
+  </si>
+  <si>
+    <t>lilach@gmail.com</t>
+  </si>
+  <si>
+    <t>054266</t>
   </si>
 </sst>
 </file>
@@ -261,7 +276,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,15 +572,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row ht="18" r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -611,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7</v>
       </c>
@@ -622,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -633,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -656,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -679,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -702,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -725,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -748,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -769,6 +784,29 @@
       </c>
       <c r="G10" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -784,9 +822,9 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row ht="18" r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,7 +898,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -934,7 +972,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
changing windows and forms
Co-Authored-By: Sapir Shemesh <shemeshsapir@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fastl\Documents\GitHub\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53281C51-E7D6-43D6-99F4-04FE0D8DB176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CAEC767B-E14C-42BA-AC57-52C0189D7A26}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="משתמשים" sheetId="1" r:id="rId1"/>
-    <sheet name="נכסים" sheetId="2" r:id="rId2"/>
+    <sheet name="משתמשים" r:id="rId1" sheetId="1"/>
+    <sheet name="נכסים" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Sapi</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -218,21 +215,9 @@
     <t>asdsad</t>
   </si>
   <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>sdfdf</t>
-  </si>
-  <si>
-    <t>dfsdf</t>
-  </si>
-  <si>
     <t>בניין</t>
   </si>
   <si>
-    <t>נתניה</t>
-  </si>
-  <si>
     <t>ירושלים</t>
   </si>
   <si>
@@ -240,12 +225,40 @@
   </si>
   <si>
     <t>קרקע</t>
+  </si>
+  <si>
+    <t>Lilach26</t>
+  </si>
+  <si>
+    <t>lilach@ngjrnj</t>
+  </si>
+  <si>
+    <t>05454</t>
+  </si>
+  <si>
+    <t>Sapir</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>shemesh@gmail.com</t>
+  </si>
+  <si>
+    <t>0526478</t>
+  </si>
+  <si>
+    <t>kus</t>
+  </si>
+  <si>
+    <t>קרקעי</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,17 +292,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -302,14 +315,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -344,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -396,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -507,21 +520,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -538,7 +551,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -590,23 +603,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row ht="18" r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -652,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7</v>
       </c>
@@ -663,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -674,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -697,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -720,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -743,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -766,12 +779,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -786,79 +799,125 @@
         <v>50</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
       <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>61</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A6" sqref="A6:Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+    <row ht="18" r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +991,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -943,13 +1002,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -961,10 +1020,10 @@
         <v>222</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L2">
         <v>222</v>
@@ -1003,10 +1062,10 @@
         <v>28</v>
       </c>
       <c r="X2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1017,70 +1076,70 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1091,10 +1150,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1112,16 +1171,16 @@
         <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1154,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1165,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1183,19 +1242,19 @@
         <v>222</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O5">
         <v>2</v>
@@ -1228,51 +1287,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>23.0</v>
       </c>
       <c r="J6" t="s">
         <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.0</v>
       </c>
       <c r="P6" t="b">
         <v>0</v>
@@ -1302,229 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="b">
-        <v>0</v>
-      </c>
-      <c r="U7" t="b">
-        <v>0</v>
-      </c>
-      <c r="V7" t="b">
-        <v>0</v>
-      </c>
-      <c r="W7" t="b">
-        <v>0</v>
-      </c>
-      <c r="X7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>222</v>
-      </c>
-      <c r="J8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" t="b">
-        <v>0</v>
-      </c>
-      <c r="U8" t="b">
-        <v>0</v>
-      </c>
-      <c r="V8" t="b">
-        <v>0</v>
-      </c>
-      <c r="W8" t="b">
-        <v>0</v>
-      </c>
-      <c r="X8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>222</v>
-      </c>
-      <c r="J9" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" t="b">
-        <v>0</v>
-      </c>
-      <c r="U9" t="b">
-        <v>0</v>
-      </c>
-      <c r="V9" t="b">
-        <v>0</v>
-      </c>
-      <c r="W9" t="b">
-        <v>0</v>
-      </c>
-      <c r="X9" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
search details - done
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fastl\Documents\GitHub\ALYS-JavaSwing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{CAEC767B-E14C-42BA-AC57-52C0189D7A26}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AC4BD6-5D65-4A56-8CBC-ACFDB9F6D023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="משתמשים" r:id="rId1" sheetId="1"/>
-    <sheet name="נכסים" r:id="rId2" sheetId="2"/>
+    <sheet name="משתמשים" sheetId="1" r:id="rId1"/>
+    <sheet name="נכסים" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
   <si>
     <t>שם משתמש</t>
   </si>
@@ -249,16 +249,12 @@
   </si>
   <si>
     <t>kus</t>
-  </si>
-  <si>
-    <t>קרקעי</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,17 +288,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -315,14 +311,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -357,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -409,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -520,21 +516,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -551,7 +547,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -603,23 +599,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="18" r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,7 +638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -665,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -676,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -687,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -710,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -733,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -756,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -779,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -802,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -825,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -848,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -871,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -895,29 +891,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:Y17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="18" r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1065,7 +1061,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1087,11 +1083,11 @@
       <c r="G3">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>222</v>
       </c>
       <c r="J3" t="s">
         <v>52</v>
@@ -1139,7 +1135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1213,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1287,15 +1283,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.0</v>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>75</v>
@@ -1303,23 +1299,23 @@
       <c r="E6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>23.0</v>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>23</v>
       </c>
       <c r="J6" t="s">
         <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
         <v>62</v>
@@ -1330,8 +1326,8 @@
       <c r="N6" t="s">
         <v>62</v>
       </c>
-      <c r="O6" t="n">
-        <v>0.0</v>
+      <c r="O6">
+        <v>0</v>
       </c>
       <c r="P6" t="b">
         <v>0</v>
@@ -1362,6 +1358,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dataController - code design
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yonatan\Documents\GitHub\ALYS-JavaSwing\ALYS-JavaSwing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B25CE7-94DA-4906-B637-66536CA8339E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B7B25CE7-94DA-4906-B637-66536CA8339E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1545" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="11385" windowWidth="21600" xWindow="5280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1545"/>
   </bookViews>
   <sheets>
-    <sheet name="משתמשים" sheetId="1" r:id="rId1"/>
-    <sheet name="נכסים" sheetId="2" r:id="rId2"/>
+    <sheet name="משתמשים" r:id="rId1" sheetId="1"/>
+    <sheet name="נכסים" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -387,6 +387,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,18 +421,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -448,10 +449,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -486,7 +487,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -538,7 +539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -649,21 +650,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -680,7 +681,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -732,15 +733,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A2:A8"/>
@@ -748,7 +749,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row ht="18.75" r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,13 +932,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -945,11 +946,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+    <row ht="18.75" r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,8 +1105,8 @@
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="n">
+        <v>2.0</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -1178,8 +1179,8 @@
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="C4" t="n">
+        <v>3.0</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -2436,8 +2437,8 @@
       <c r="B21" s="2">
         <v>23.525641025641001</v>
       </c>
-      <c r="C21">
-        <v>3</v>
+      <c r="C21" t="n">
+        <v>4.0</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -4064,8 +4065,8 @@
       <c r="B43" s="2">
         <v>48.532634032634398</v>
       </c>
-      <c r="C43">
-        <v>1</v>
+      <c r="C43" t="n">
+        <v>2.0</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -4138,8 +4139,8 @@
       <c r="B44" s="2">
         <v>49.574592074592502</v>
       </c>
-      <c r="C44">
-        <v>2</v>
+      <c r="C44" t="n">
+        <v>3.0</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -4872,6 +4873,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>